<commit_message>
flujo de compra de plan agregado
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\IdeaProjects\MovilExitoAndroid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\IdeaProjects\MovilExitoAndroid18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912BCE3E-A550-4084-9DF1-317490A48914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291B27D3-883B-479B-B1A8-79D25E586179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{569054DB-B792-4226-B685-BECA8AA6D15D}"/>
+    <workbookView xWindow="-240" yWindow="0" windowWidth="29040" windowHeight="15480" activeTab="1" xr2:uid="{569054DB-B792-4226-B685-BECA8AA6D15D}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro" sheetId="1" r:id="rId1"/>
+    <sheet name="Planform" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Datos</t>
   </si>
@@ -46,6 +47,9 @@
   </si>
   <si>
     <t>cabraLoca66</t>
+  </si>
+  <si>
+    <t>dhaenerhys@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -410,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C28B63C-C663-40D2-97BF-CE3B1DB573DE}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,4 +459,47 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E061AF14-270D-4277-B539-9707C7A0026B}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3004442525</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1001828778</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{48B5988C-AAF3-40EC-BB12-B2C518A2F88D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>